<commit_message>
Se reorganizan archivos para diferentes versiones de HMI.
</commit_message>
<xml_diff>
--- a/Programas/parametros.xlsx
+++ b/Programas/parametros.xlsx
@@ -1,35 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="PID" sheetId="1" r:id="rId1"/>
+    <sheet name="Temp" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>minimo</t>
-  </si>
-  <si>
-    <t>maximo</t>
-  </si>
-  <si>
-    <t>deltamv</t>
-  </si>
-  <si>
-    <t>scantime</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -70,7 +52,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -80,7 +62,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -366,80 +348,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F9"/>
+  <dimension ref="B2:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C1">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>5400</v>
+      </c>
+      <c r="D2">
+        <v>7200</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>200</v>
+      </c>
+      <c r="D3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>2400</v>
+      </c>
+      <c r="D4">
         <v>1600</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C2">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6">
         <v>1000</v>
       </c>
-      <c r="F2">
-        <v>5360</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C3">
-        <v>2200</v>
-      </c>
-      <c r="F3">
-        <v>20500</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>892</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <v>300</v>
-      </c>
-      <c r="F5">
-        <v>1544</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C6">
+      <c r="D6">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="D7">
         <v>0</v>
       </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9">
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>795</v>
+      </c>
+      <c r="D9">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>3000</v>
+      </c>
+      <c r="D10">
         <v>3000</v>
       </c>
     </row>
@@ -450,24 +435,36 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>704</v>
+      </c>
+      <c r="D2">
+        <v>9.94</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1544</v>
+      </c>
+      <c r="D3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>